<commit_message>
Update of the TODO list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\Git_DRomics\DRomics\share\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\Git_DRomics\DRomics\share\techdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t xml:space="preserve">5.Corriger la gestion des NA dans drcfit (cf. données photosynthesis Diuron). Gérer ligne 77 de drcfit et la suite (pb quand on récupère les résidus qui ne sont pas de la même longueur que les rangs des observations). Vérifier que cela ne pose pas de souci avant. </t>
   </si>
@@ -153,9 +153,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>28. Donner diverses options d’un plot de sensibilité par pathway (boxplot, autre stat résumées…) – fonction englobante sensitivityplot</t>
-  </si>
-  <si>
     <t>priorités</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>48. Essayer de mettre le filtre sur les résidus meantrend) avant la sélection car parfois on doit enlever des items pour lesquels un des modèle allait. A DISCUTER AVCE ELISE !</t>
   </si>
   <si>
-    <t>49. Ajouter un argument facetby2 à bmdplotwithgradient pour mettre un facteur en ligne et un en colonne avec facet_grid()</t>
-  </si>
-  <si>
     <t>50. Dans la vignette écrire plus explicitement qu’on peut rentrer le jeu de données directement en objet R</t>
   </si>
   <si>
@@ -252,9 +246,6 @@
     <t>52. Changer le jeu de données exemple RNAseq, mettre un de Gwinn avec plus de concentrations</t>
   </si>
   <si>
-    <t>53. tenter d'éviter les pbs de pics trop haut (ou trop bas) avec LGP notamment</t>
-  </si>
-  <si>
     <t>54. Mettre un message si quelquun fixe minBMD plus grand que la plus petite conc non nulle</t>
   </si>
   <si>
@@ -264,7 +255,25 @@
     <t>56. faire un boostrap avec modèle libre pour avoir notamment l'incertitude sur la trend</t>
   </si>
   <si>
-    <t>57. ajout de labels au plot de bmdboot</t>
+    <t>49. Ajouter un argument facetby2 à bmdplotwithgradient et curvesplot pour mettre un facteur en ligne et un en colonne avec facet_grid()</t>
+  </si>
+  <si>
+    <t>58. ajouter une fonction trendplot (cf. article diuron)</t>
+  </si>
+  <si>
+    <t>A + ML</t>
+  </si>
+  <si>
+    <t>53. tenter d'éviter les pbs de pics trop haut (ou trop bas) avec LGP notamment - contraindre largeur de la gaussienne à ne pas être trop petite par rapport à l'espace entre deux concentrations</t>
+  </si>
+  <si>
+    <t>57. ajout de labels au plot de bmdboot - impossible car dans ce step 5 on n'a pas l'annotation. Plutôt faire une fonction bmdplotwithCI qui appelle ECDFplotwithCI et donne la possibilité de mettre des labels, avec un facetby et un facetby2</t>
+  </si>
+  <si>
+    <t>top priorités</t>
+  </si>
+  <si>
+    <t>28. Donner diverses options d’un plot de sensibilité par pathway (boxplot, autre stat résumées…) – fonction englobante sensitivityplot  avec plusieurs groupes (ex. article diuron) en résolvant le pb de l'ordre des items</t>
   </si>
 </sst>
 </file>
@@ -295,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,8 +317,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -317,11 +338,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -334,12 +370,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -616,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -627,7 +681,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
@@ -745,52 +799,52 @@
     </row>
     <row r="24" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -801,38 +855,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="108.77734375" customWidth="1"/>
+    <col min="1" max="1" width="126.5546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
       </c>
+      <c r="D2" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
@@ -840,7 +897,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B4" t="s">
@@ -848,7 +905,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
@@ -856,96 +913,108 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>33</v>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>45</v>
+      <c r="A10" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="21" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>66</v>
-      </c>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -972,27 +1041,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1025,7 +1094,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add of the argument facetby2 in curvesplot() and bmdpltwithgradient()
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="done" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t xml:space="preserve">5.Corriger la gestion des NA dans drcfit (cf. données photosynthesis Diuron). Gérer ligne 77 de drcfit et la suite (pb quand on récupère les résidus qui ne sont pas de la même longueur que les rangs des observations). Vérifier que cela ne pose pas de souci avant. </t>
   </si>
@@ -304,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,6 +326,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -383,6 +389,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,19 +842,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -855,10 +873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,61 +974,56 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>63</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>60</v>
+      <c r="A18" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="A22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add of the function trendplot()
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="done" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t xml:space="preserve">5.Corriger la gestion des NA dans drcfit (cf. données photosynthesis Diuron). Gérer ligne 77 de drcfit et la suite (pb quand on récupère les résidus qui ne sont pas de la même longueur que les rangs des observations). Vérifier que cela ne pose pas de souci avant. </t>
   </si>
@@ -678,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A46" sqref="A43:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,6 +865,14 @@
         <v>30</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -873,10 +881,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,7 +983,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="10" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1016,14 +1024,6 @@
       <c r="A20" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor correction and update of the TODO list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -273,7 +273,7 @@
     <t>top priorités</t>
   </si>
   <si>
-    <t>28. Donner diverses options d’un plot de sensibilité par pathway (boxplot, autre stat résumées…) – fonction englobante sensitivityplot  avec plusieurs groupes (ex. article diuron) en résolvant le pb de l'ordre des items</t>
+    <t>28. Donner diverses options d’un plot de sensibilité par pathway (boxplot, autre stat résumées…) – fonction englobante sensitivityplot  avec plusieurs groupes (ex. article diuron) en résolvant le pb de l'ordre des items - FAIT EN PARTIE - A VALIDER PAR FLORIANE ET ELISE</t>
   </si>
 </sst>
 </file>
@@ -883,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update of the TODO list and of the cheatsheet
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="done" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t xml:space="preserve">5.Corriger la gestion des NA dans drcfit (cf. données photosynthesis Diuron). Gérer ligne 77 de drcfit et la suite (pb quand on récupère les résidus qui ne sont pas de la même longueur que les rangs des observations). Vérifier que cela ne pose pas de souci avant. </t>
   </si>
@@ -165,12 +165,6 @@
     <t>31. programmation défensive si nb d’items trop petit sur le plot de sensibilité par groupe –mais quoi faire exactement ? Quantile fait de l’interpolation linéaire et sort un résultat quoiqu’il arrive</t>
   </si>
   <si>
-    <t xml:space="preserve">32. Faire une cheat sheet de DRomics – recto sur site de DRomics </t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>33. Changer par défaut la représentation des boxplots des données pour qu’elle soit moins lourde (pour le moment géré juste avec range passé dans le … de la fonction plot</t>
   </si>
   <si>
@@ -237,21 +231,12 @@
     <t>48. Essayer de mettre le filtre sur les résidus meantrend) avant la sélection car parfois on doit enlever des items pour lesquels un des modèle allait. A DISCUTER AVCE ELISE !</t>
   </si>
   <si>
-    <t>50. Dans la vignette écrire plus explicitement qu’on peut rentrer le jeu de données directement en objet R</t>
-  </si>
-  <si>
     <t>51. Ajouter les mots clefs transcriptomics, proteomics, metabolomics, toxicogenomics, multi-omics… dans le package</t>
   </si>
   <si>
     <t>52. Changer le jeu de données exemple RNAseq, mettre un de Gwinn avec plus de concentrations</t>
   </si>
   <si>
-    <t>54. Mettre un message si quelquun fixe minBMD plus grand que la plus petite conc non nulle</t>
-  </si>
-  <si>
-    <t>55. Proposer une figure par groupe avec médiane et intervalle interquartile, ou moyenne et 2 SD ? + indice de similarité de forme ?</t>
-  </si>
-  <si>
     <t>56. faire un boostrap avec modèle libre pour avoir notamment l'incertitude sur la trend</t>
   </si>
   <si>
@@ -267,13 +252,28 @@
     <t>53. tenter d'éviter les pbs de pics trop haut (ou trop bas) avec LGP notamment - contraindre largeur de la gaussienne à ne pas être trop petite par rapport à l'espace entre deux concentrations</t>
   </si>
   <si>
-    <t>57. ajout de labels au plot de bmdboot - impossible car dans ce step 5 on n'a pas l'annotation. Plutôt faire une fonction bmdplotwithCI qui appelle ECDFplotwithCI et donne la possibilité de mettre des labels, avec un facetby et un facetby2</t>
-  </si>
-  <si>
     <t>top priorités</t>
   </si>
   <si>
     <t>28. Donner diverses options d’un plot de sensibilité par pathway (boxplot, autre stat résumées…) – fonction englobante sensitivityplot  avec plusieurs groupes (ex. article diuron) en résolvant le pb de l'ordre des items - FAIT EN PARTIE - A VALIDER PAR FLORIANE ET ELISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32. Faire une cheat sheet de DRomics – recto à mettre sur site de DRomics </t>
+  </si>
+  <si>
+    <t>50. Dans la vignette écrire plus explicitement qu’on peut rentrer le jeu de données directement en objet R. C'était déjà écrit. J'ai juste ajouté un passage à la ligne et l'ai mis aussi dans la cheat sheet.</t>
+  </si>
+  <si>
+    <t>54. Mettre un message si quelqu'un fixe minBMD plus grand que la plus petite conc non nulle</t>
+  </si>
+  <si>
+    <t>57. ajout de labels au plot de bmdboot - impossible car dans ce step 5 on n'a pas l'annotation. Plutôt faire une fonction bmdplotwithCI qui appelle ECDFplotwithCI et donne la possibilité de mettre des labels, avec un facetby et un facetby2 - j'ai fait une fonction bmdplot poru gérer cela</t>
+  </si>
+  <si>
+    <t>55. Proposer une figure par groupe avec médiane et intervalle interquartile, ou moyenne et 2 SD ? + indice de similarité de forme ? FAIT en partie dans senitivityplot() - A COMPLETER ?</t>
+  </si>
+  <si>
+    <t>58. programmation défensive sur toutes les fonctions avec extendedres en input (vérification que tousles arguments sont en colonne)</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -393,6 +393,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A46" sqref="A43:A46"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,7 +696,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
@@ -809,57 +814,57 @@
     </row>
     <row r="24" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>30</v>
@@ -867,9 +872,49 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="15" t="s">
         <v>30</v>
       </c>
     </row>
@@ -881,10 +926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,7 +956,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -948,81 +993,61 @@
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="B12" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1069,12 +1094,12 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1107,7 +1132,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of the TODOlist
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="done" sheetId="1" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>48. Essayer de mettre le filtre sur les résidus meantrend) avant la sélection car parfois on doit enlever des items pour lesquels un des modèle allait. A DISCUTER AVCE ELISE !</t>
   </si>
   <si>
-    <t>51. Ajouter les mots clefs transcriptomics, proteomics, metabolomics, toxicogenomics, multi-omics… dans le package</t>
-  </si>
-  <si>
     <t>52. Changer le jeu de données exemple RNAseq, mettre un de Gwinn avec plus de concentrations</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>58. programmation défensive sur toutes les fonctions avec extendedres en input (vérification que tousles arguments sont en colonne)</t>
+  </si>
+  <si>
+    <t>51. Ajouter keywords : dose response modelling, benchmark dose (BMD), environmental risk assessment, transcriptomics, proteomics, metabolomics, toxicogenomics, multi-omics… dans le readme du GitHub et sur le site web de DRomics</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -864,7 +864,7 @@
     </row>
     <row r="36" spans="1:2" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>30</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
         <v>30</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="38" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>30</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>30</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>30</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="41" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>30</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>30</v>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,7 +956,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -993,7 +993,7 @@
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>30</v>
@@ -1019,27 +1019,27 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating of the todo list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>59. enlever l'argument sigmoid.model de drcfit (donc l'utilisation possible du modèle log_probit, mais sans l'enlever completement pour nous) car c'est de nature à perturber l'utilisateur qui croit qu'il eut choisir le modele (ex. Stefan)</t>
+  </si>
+  <si>
+    <t>60. add of the Rager in situ data set</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,7 +364,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -430,6 +439,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -780,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="A44" sqref="A44:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,6 +1036,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1033,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1147,12 +1168,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tasks in the TODO list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -261,9 +261,6 @@
     <t>52. Changer le jeu de données exemple RNAseq, mettre un de Gwinn avec plus de concentrations</t>
   </si>
   <si>
-    <t>53. tenter d'éviter les pbs de pics trop haut (ou trop bas) avec LGP notamment - contraindre largeur de la gaussienne à ne pas être trop petite par rapport à l'espace entre deux concentrations</t>
-  </si>
-  <si>
     <t>55. Proposer une figure par groupe avec médiane et intervalle interquartile, ou moyenne et 2 SD ? + indice de similarité de forme ? FAIT en partie dans senitivityplot() - A COMPLETER ?</t>
   </si>
   <si>
@@ -304,6 +301,15 @@
   </si>
   <si>
     <t>61. ajouter l'argument range aux fonctions de plot des données importées</t>
+  </si>
+  <si>
+    <t>53. tenter d'éviter les pbs de pics trop haut (ou trop bas) avec LGP notamment - contraindre largeur de la gaussienne à ne pas être trop petite par rapport à l'espace entre deux concentrations DIFFICILE ! Plutôt mettre un AIC infini si le pic dépasse le min ou le max</t>
+  </si>
+  <si>
+    <t>63 regarder le souci avec l'échelle des y qui change d'une page à l'autre dans plotfit2pdf (en résidus si outliers ou non notamment)</t>
+  </si>
+  <si>
+    <t>62. ajouter un etst sur les outliers pour les cas excessifs cf. transcripto rainettes 2018</t>
   </si>
 </sst>
 </file>
@@ -810,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -1053,7 +1059,7 @@
     </row>
     <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>35</v>
@@ -1061,7 +1067,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>51</v>
@@ -1075,7 +1081,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -1167,12 +1173,12 @@
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
@@ -1180,20 +1186,30 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1225,27 +1241,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1269,17 +1285,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificatin on all the importation functions to prevent the calculation of BMDs by extrapolation when there is no dose at 0 in the data - repercussion in the Shiny app. still to handle,
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -303,9 +303,6 @@
     <t>61. ajouter l'argument range aux fonctions de plot des données importées</t>
   </si>
   <si>
-    <t>53. tenter d'éviter les pbs de pics trop haut (ou trop bas) avec LGP notamment - contraindre largeur de la gaussienne à ne pas être trop petite par rapport à l'espace entre deux concentrations DIFFICILE ! Plutôt mettre un AIC infini si le pic dépasse le min ou le max</t>
-  </si>
-  <si>
     <t>63 regarder le souci avec l'échelle des y qui change d'une page à l'autre dans plotfit2pdf (en résidus si outliers ou non notamment)</t>
   </si>
   <si>
@@ -315,13 +312,16 @@
     <t>65. changer le nom adjpvalue en qvalue dans les sorties pour que ce soit plus clair !!! (pas clair la tricherie dans Rager 2017)</t>
   </si>
   <si>
-    <t>64. sur les données in situ de type Rager 2017 avec les plus faibles doses loin du zéro. Si on n'a pas de dose à zéro, demander à l'utilisateur d'indiquer une valeur seuil en dessous de laquelle on considère que la dose est négligeable, du niveau du contrôle et fixer les doses inférieures ou égales à 0</t>
-  </si>
-  <si>
     <t>66. éliminer en amont, avant comparason des AICs les pics qui dépassent la gamme du signal observé</t>
   </si>
   <si>
     <t>67. tenter de fixer le f à 0 pour les modèles Gauss-probit et log-Gauss-probit, sans réajuster ou en réajustant à partir des mêmes valeurs, et garder le probit ou log-probit s'il est meilleur en AIC</t>
+  </si>
+  <si>
+    <t>53. tenter d'éviter les pbs de pics trop haut (ou trop bas) avec LGP notamment - contraindre largeur de la gaussienne à ne pas être trop petite par rapport à l'espace entre deux concentrations DIFFICILE ! Plutôt mettre un AIC infini si le pic dépasse le min ou le max (see 66)</t>
+  </si>
+  <si>
+    <t>64. sur les données in situ de type Rager 2017 avec les plus faibles doses loin du zéro. Si on n'a pas de dose à zéro, demander à l'utilisateur de mettre à 0 les doses qu'ils considère correspondre au niveau de base (background) pour éviter que la BMD soit calculée par extrapolation san contrôle du modèle par les données à la dose 0</t>
   </si>
 </sst>
 </file>
@@ -352,7 +352,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +399,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -455,9 +461,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -476,6 +479,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -826,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,10 +1076,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1083,6 +1089,27 @@
       </c>
       <c r="B45" s="10" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1093,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1151,7 +1178,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1185,72 +1212,54 @@
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>73</v>
+      <c r="B18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1321,21 +1330,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="110.109375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="110.109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mise à jour de la TODO list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="done" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1103,6 +1103,9 @@
       <c r="A47" s="21" t="s">
         <v>77</v>
       </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
@@ -1122,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
put new arguments of drcfit enablesfequal0 to FALSE as there is still a BUG in the bmdboot for biphasic models with f = 0
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -333,6 +333,13 @@
   </si>
   <si>
     <t>69. ajouter la possibilité d'ajouter sur le plot d'un drcfit les BMD en ajoutant un argument avec la sortie de bmdcalc voire même celle de bmdboot pour mettre les bornes des IC</t>
+  </si>
+  <si>
+    <t>70. Régler le message d'erreur dans le bootstrap sur jeu de données Olivier 
+Error in if (y0 &gt; threshold &amp; threshold &gt; yext &amp; xext != 0) { : 
+  valeur manquante là où TRUE / FALSE est requis
+De plus : There were 50 or more warnings (use warnings() to see the first 50)
+en attendant je remets les enablesfequa0 à FALSE par défaut</t>
   </si>
 </sst>
 </file>
@@ -363,7 +370,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,6 +425,12 @@
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -446,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -493,6 +506,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1142,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1287,6 +1303,11 @@
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of the toto list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -294,9 +294,6 @@
     <t>27. Retravailler le line.size de bmdplotwithgradient: Aurélie a essayé  sans succès. On laisse tomber</t>
   </si>
   <si>
-    <t>61. ajouter l'argument range aux fonctions de plot des données importées</t>
-  </si>
-  <si>
     <t>63 regarder le souci avec l'échelle des y qui change d'une page à l'autre dans plotfit2pdf (en résidus si outliers ou non notamment)</t>
   </si>
   <si>
@@ -310,10 +307,6 @@
   </si>
   <si>
     <t>64. sur les données in situ de type Rager 2017 avec les plus faibles doses loin du zéro. Si on n'a pas de dose à zéro, demander à l'utilisateur de mettre à 0 les doses qu'ils considère correspondre au niveau de base (background) pour éviter que la BMD soit calculée par extrapolation san contrôle du modèle par les données à la dose 0</t>
-  </si>
-  <si>
-    <t>65. changer le nom adjpvalue en qvalue dans les sorties pour que ce soit plus clair !!! (pas clair la tricherie dans Rager 2017)
-TO DISCUSS ALL TOGETHER BEFORE</t>
   </si>
   <si>
     <t>56. faire un boostrap avec modèle libre pour avoir notamment l'incertitude sur la trend - 
@@ -321,25 +314,25 @@
 on est content si c'est 100%</t>
   </si>
   <si>
+    <t>67. tenter de fixer le f à 0 pour les modèles Gauss-probit et log-Gauss-probit, sans réajuster ou en réajustant à partir des mêmes valeurs, et garder le probit ou log-probit s'il est meilleur en AIC: réajustement systématique avec f = 0  du modèle si GP5p ou lGP5p et retenue du modèle simplifié sur critère d'information meilleur</t>
+  </si>
+  <si>
+    <t>68. ajouter un échantillon du jeu de données de Rager 2017 qu'on appelera arsenic</t>
+  </si>
+  <si>
+    <t>61. ajouter l'argument range (à passer à boxplot) aux fonctions de plot des données importées</t>
+  </si>
+  <si>
+    <t>69. ajouter la possibilité d'ajouter sur le plot d'un drcfit les BMD en ajoutant un argument avec la sortie de bmdcalc voire même celle de bmdboot pour mettre les bornes des IC - done in plot.drcfit to do in plotfit2pdf</t>
+  </si>
+  <si>
+    <t>65. changer le nom adjpvalue en qvalue dans les sorties pour que ce soit plus clair !!! (pas clair la tricherie dans Rager 2017)
+TO DISCUSS ALL TOGETHER BEFORE acompagner les utilisateurs à un cgt dans la prochane release - message au chargement du package !</t>
+  </si>
+  <si>
     <t>60. add of the Rager in situ data set - est-ce raisonnable vu qu'on ne ressort rien avec un FDR raisonnable ?
 Prendre un sous-ensemble déjà trié sur le fold change par exemple (un peu triché !)
-A DISCUTER !!!</t>
-  </si>
-  <si>
-    <t>67. tenter de fixer le f à 0 pour les modèles Gauss-probit et log-Gauss-probit, sans réajuster ou en réajustant à partir des mêmes valeurs, et garder le probit ou log-probit s'il est meilleur en AIC: réajustement systématique avec f = 0  du modèle si GP5p ou lGP5p et retenue du modèle simplifié sur critère d'information meilleur</t>
-  </si>
-  <si>
-    <t>68. ajouter un échantillon du jeu de données de Rager 2017 qu'on appelera arsenic</t>
-  </si>
-  <si>
-    <t>69. ajouter la possibilité d'ajouter sur le plot d'un drcfit les BMD en ajoutant un argument avec la sortie de bmdcalc voire même celle de bmdboot pour mettre les bornes des IC</t>
-  </si>
-  <si>
-    <t>70. Régler le message d'erreur dans le bootstrap sur jeu de données Olivier 
-Error in if (y0 &gt; threshold &amp; threshold &gt; yext &amp; xext != 0) { : 
-  valeur manquante là où TRUE / FALSE est requis
-De plus : There were 50 or more warnings (use warnings() to see the first 50)
-en attendant je remets les enablesfequa0 à FALSE par défaut</t>
+NON : AJOUT d'un sous jeu de données d'Olivier en RNAseqinsitusample.txt + test des modifs in situ sur sa base</t>
   </si>
 </sst>
 </file>
@@ -370,7 +363,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,12 +418,6 @@
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -459,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -506,9 +493,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1120,7 +1104,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>35</v>
@@ -1128,7 +1112,7 @@
     </row>
     <row r="47" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -1136,7 +1120,7 @@
     </row>
     <row r="48" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>35</v>
@@ -1144,7 +1128,7 @@
     </row>
     <row r="49" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
         <v>35</v>
@@ -1158,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,17 +1242,17 @@
     </row>
     <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1276,7 +1260,7 @@
     </row>
     <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
@@ -1284,12 +1268,12 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -1297,18 +1281,19 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>81</v>
-      </c>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+    </row>
+    <row r="22" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add of an insitu data sample to check the new options to cope pb with such data and correction of one BUG when using background on RNAseq in situ data
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -317,13 +317,7 @@
     <t>67. tenter de fixer le f à 0 pour les modèles Gauss-probit et log-Gauss-probit, sans réajuster ou en réajustant à partir des mêmes valeurs, et garder le probit ou log-probit s'il est meilleur en AIC: réajustement systématique avec f = 0  du modèle si GP5p ou lGP5p et retenue du modèle simplifié sur critère d'information meilleur</t>
   </si>
   <si>
-    <t>68. ajouter un échantillon du jeu de données de Rager 2017 qu'on appelera arsenic</t>
-  </si>
-  <si>
     <t>61. ajouter l'argument range (à passer à boxplot) aux fonctions de plot des données importées</t>
-  </si>
-  <si>
-    <t>69. ajouter la possibilité d'ajouter sur le plot d'un drcfit les BMD en ajoutant un argument avec la sortie de bmdcalc voire même celle de bmdboot pour mettre les bornes des IC - done in plot.drcfit to do in plotfit2pdf</t>
   </si>
   <si>
     <t>65. changer le nom adjpvalue en qvalue dans les sorties pour que ce soit plus clair !!! (pas clair la tricherie dans Rager 2017)
@@ -333,6 +327,9 @@
     <t>60. add of the Rager in situ data set - est-ce raisonnable vu qu'on ne ressort rien avec un FDR raisonnable ?
 Prendre un sous-ensemble déjà trié sur le fold change par exemple (un peu triché !)
 NON : AJOUT d'un sous jeu de données d'Olivier en RNAseqinsitusample.txt + test des modifs in situ sur sa base</t>
+  </si>
+  <si>
+    <t>68. ajouter la possibilité d'ajouter sur le plot d'un drcfit les BMD en ajoutant un argument avec la sortie de bmdcalc voire même celle de bmdboot pour mettre les bornes des IC - done in plot.drcfit to do in plotfit2pdf</t>
   </si>
 </sst>
 </file>
@@ -843,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,6 +1131,22 @@
         <v>35</v>
       </c>
     </row>
+    <row r="50" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1142,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1245,55 +1258,40 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-    </row>
-    <row r="22" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+    </row>
+    <row r="20" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
one add in the TODO list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>68. ajouter la possibilité d'ajouter sur le plot d'un drcfit les BMD en ajoutant un argument avec la sortie de bmdcalc voire même celle de bmdboot pour mettre les bornes des IC - done in plot.drcfit to do in plotfit2pdf</t>
+  </si>
+  <si>
+    <t>69. mettre un warning ou interdire l'utilisation de l'anova si pas au moins 2 ou 3 réplcats par groupe</t>
   </si>
 </sst>
 </file>
@@ -842,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
@@ -1157,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1285,6 +1288,11 @@
       </c>
       <c r="B17" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update news and todo list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="done" sheetId="1" r:id="rId1"/>
@@ -294,9 +294,6 @@
     <t>27. Retravailler le line.size de bmdplotwithgradient: Aurélie a essayé  sans succès. On laisse tomber</t>
   </si>
   <si>
-    <t>63 regarder le souci avec l'échelle des y qui change d'une page à l'autre dans plotfit2pdf (en résidus si outliers ou non notamment)</t>
-  </si>
-  <si>
     <t>62. ajouter un test sur les outliers pour les cas excessifs cf. transcripto rainettes 2018 (implémenter sur chaque item, dès la vérification des données, sans prendre en compte la dose-réponse, une détection basée sur le Z-score modifié de Iglewicz, B., &amp; Hoaglin, D. C. (1993). How to detect and handle outliers (Vol. 16). Asq Press. (1115 citations google scholar))</t>
   </si>
   <si>
@@ -328,12 +325,16 @@
     <t>68. ajouter la possibilité d'ajouter sur le plot d'un drcfit les BMD en ajoutant un argument avec la sortie de bmdcalc voire même celle de bmdboot pour mettre les bornes des IC - done in plot.drcfit to do in plotfit2pdf</t>
   </si>
   <si>
-    <t>65. changer le nom adjpvalue en qvalue dans les sorties pour que ce soit plus clair !!! (pas clair la tricherie dans Rager 2017)
-Non car personne ne connait en ecotox, mais a mentionner dans l'aide</t>
-  </si>
-  <si>
     <t>69. mettre un warning ou interdire l'utilisation de l'anova si pas au moins 2 ou 3 réplicats par groupe
 interdire anova si trop de doses avec un seul réplicat (ex. superieur à 50%)</t>
+  </si>
+  <si>
+    <t>65. changer le nom adjpvalue en qvalue dans les sorties pour que ce soit plus clair !!! (pas clair la tricherie dans Rager 2017)
+Non car personne ne connait en ecotox, mais a mentionner dans l'aide - FAIT dans ade de itemselect</t>
+  </si>
+  <si>
+    <t>63 regarder le souci avec l'échelle des y qui change d'une page à l'autre dans plotfit2pdf (en résidus si outliers ou non notamment)
+not possible -&gt; residuals calculated within the function called in the loop</t>
   </si>
 </sst>
 </file>
@@ -364,7 +365,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,12 +410,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
@@ -447,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -490,10 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -844,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,15 +1097,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="21" t="s">
-        <v>72</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -1121,7 +1113,7 @@
     </row>
     <row r="48" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>35</v>
@@ -1129,7 +1121,7 @@
     </row>
     <row r="49" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
         <v>35</v>
@@ -1137,7 +1129,7 @@
     </row>
     <row r="50" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>35</v>
@@ -1145,10 +1137,34 @@
     </row>
     <row r="51" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B51" t="s">
-        <v>35</v>
+      <c r="B53" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1159,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1259,12 +1275,12 @@
     </row>
     <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
@@ -1272,41 +1288,27 @@
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18"/>
     </row>
     <row r="19" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-    </row>
-    <row r="20" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
+      <c r="A19" s="9"/>
+      <c r="B19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
update workflow2 and TODO list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="done" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -335,6 +335,15 @@
   <si>
     <t>63 regarder le souci avec l'échelle des y qui change d'une page à l'autre dans plotfit2pdf (en résidus si outliers ou non notamment)
 not possible -&gt; residuals calculated within the function called in the loop</t>
+  </si>
+  <si>
+    <t>70. look at the problem of format of the last page of the pdf file with the argument BMDoutput (cf. ex. transcripto 2018)</t>
+  </si>
+  <si>
+    <t>71. put an example to help the formating of data especially in a R object</t>
+  </si>
+  <si>
+    <t>72. Add a function associated with sensitivityplot to get the numrical summaries and to do other plots (boxplots)</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,6 +423,12 @@
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -442,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -486,6 +501,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -838,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -1177,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="A16:B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1295,16 +1313,26 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+      <c r="A17" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="B17" s="17"/>
     </row>
     <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18"/>
+      <c r="A18" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>

</xml_diff>

<commit_message>
further update of the todo list
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\GitHub_DRomics\DRomics\share\techdoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\GitHub\DRomics\share\techdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA7A003-34D7-478F-B8F6-E471C2A9629D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="done" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -363,11 +364,23 @@
   <si>
     <t>76. modifier la fonction curvesplot pour ajouter une normalisation sur maxydiff</t>
   </si>
+  <si>
+    <t>79. modification of examples for DRomicsInterpreter by adding BMD_xfold</t>
+  </si>
+  <si>
+    <t>80. find a way to give an example in the DRomicsInterpreter shiny app</t>
+  </si>
+  <si>
+    <t>81. add Danio rerio data in the package as another example for the functions for Dromics results interpretation (without enrichment and/or with outlier elimination as in the paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82. Implement a way to eliminate batch effect (or another factor) or to take it into account with the selection and the modeling </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -872,19 +885,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="113.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="113.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -892,167 +905,167 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1060,7 +1073,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1068,7 +1081,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
@@ -1076,7 +1089,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
@@ -1084,7 +1097,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
@@ -1092,7 +1105,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>41</v>
       </c>
@@ -1100,7 +1113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>42</v>
       </c>
@@ -1108,7 +1121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -1116,7 +1129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
         <v>66</v>
       </c>
@@ -1124,7 +1137,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
         <v>67</v>
       </c>
@@ -1132,7 +1145,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
         <v>69</v>
       </c>
@@ -1140,7 +1153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="20" t="s">
         <v>70</v>
       </c>
@@ -1148,7 +1161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>71</v>
       </c>
@@ -1156,7 +1169,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
         <v>73</v>
       </c>
@@ -1164,7 +1177,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
         <v>75</v>
       </c>
@@ -1172,7 +1185,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
         <v>76</v>
       </c>
@@ -1180,7 +1193,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>78</v>
       </c>
@@ -1188,7 +1201,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>77</v>
       </c>
@@ -1196,7 +1209,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
         <v>79</v>
       </c>
@@ -1211,19 +1224,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="126.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="126.54296875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>44</v>
       </c>
@@ -1234,7 +1247,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
@@ -1245,7 +1258,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>48</v>
       </c>
@@ -1253,7 +1266,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>49</v>
       </c>
@@ -1261,7 +1274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>50</v>
       </c>
@@ -1269,7 +1282,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>52</v>
       </c>
@@ -1277,27 +1290,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>57</v>
       </c>
@@ -1305,7 +1318,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>82</v>
       </c>
@@ -1313,7 +1326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>72</v>
       </c>
@@ -1321,7 +1334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>74</v>
       </c>
@@ -1329,7 +1342,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>68</v>
       </c>
@@ -1337,7 +1350,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>80</v>
       </c>
@@ -1345,13 +1358,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>81</v>
       </c>
       <c r="B17" s="17"/>
     </row>
-    <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>83</v>
       </c>
@@ -1359,7 +1372,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>84</v>
       </c>
@@ -1367,7 +1380,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>85</v>
       </c>
@@ -1375,7 +1388,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>88</v>
       </c>
@@ -1383,7 +1396,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
         <v>89</v>
       </c>
@@ -1391,14 +1404,46 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
         <v>87</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="18" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1408,19 +1453,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -1428,27 +1473,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1460,29 +1505,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="110.140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="110.1796875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
minor changes following discussion with Aurélie
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\GitHub\DRomics\share\techdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0B5304-E7EB-4017-B9A2-ADAEEC2CEF66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BEC5E2-674D-462B-884F-006E795192DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="99">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -356,9 +356,6 @@
     <t>81. add Danio rerio data in the package as another example for the functions for Dromics results interpretation (without enrichment and/or with outlier elimination as in the paper</t>
   </si>
   <si>
-    <t>83. try to make the size scale of nb_of_items print only integer values in sensitivityplot and trendplot</t>
-  </si>
-  <si>
     <t>84. ajouter dans le package une fonction de visualisation de l'ensemble des données en ACP pour voir la cohérence et détecter d'éventuels outliers</t>
   </si>
   <si>
@@ -380,13 +377,19 @@
     <t>75. ajouter aux sorties de drcfit une colonne maxychange qui sera la diff max absolue entre y et t0 dans la gamme étudiée - penser à mettre à jour informations_bmdcalc_results.txt</t>
   </si>
   <si>
-    <t>76. modifier la fonction curvesplot pour ajouter une normalisation sur maxydiff + option ajoutée à Shiny</t>
-  </si>
-  <si>
-    <t>82. Implement a way to eliminate batch effect (or another factor) or to take it into account with the selection and the modeling using ComBat or ComBatseq from sva package (specified as suggested in the description as for parallel computation)</t>
-  </si>
-  <si>
-    <t>ML puis A ?</t>
+    <t>ML +A</t>
+  </si>
+  <si>
+    <t>76. modifier la fonction curvesplot et bmdplotwithgradient pour ajouter une normalisation sur maxydiff + option ajoutée à Shiny</t>
+  </si>
+  <si>
+    <t>82. Give an example to show how to eliminate batch effect (or another factor) or to take it into account with the selection and the modeling using ComBat or ComBatseq from sva package (specified as suggested in the description as for parallel computation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ML </t>
+  </si>
+  <si>
+    <t>83. try to make the size scale of nb_of_items print only integer values in sensitivityplot and trendplot (cf. fig vignette 3.3) - pb ggplot</t>
   </si>
 </sst>
 </file>
@@ -902,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="A57" sqref="A57:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1233,6 +1236,30 @@
         <v>51</v>
       </c>
     </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1241,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,7 +1387,7 @@
     </row>
     <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1368,7 +1395,7 @@
     </row>
     <row r="16" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>51</v>
@@ -1376,7 +1403,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>35</v>
@@ -1384,31 +1411,31 @@
     </row>
     <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>92</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="21" t="s">
-        <v>94</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>83</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>35</v>
@@ -1416,74 +1443,50 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>93</v>
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add of the function formatdata4DRomics and change of the format of the data zebraf to give an example of correction for batch effect
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\GitHub\DRomics\share\techdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BEC5E2-674D-462B-884F-006E795192DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182DE02C-4373-4B71-B07D-AD9A39A1FB4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:B57"/>
+    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1260,6 +1260,22 @@
         <v>35</v>
       </c>
     </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A59" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1268,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1401,91 +1417,75 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B18" t="s">
-        <v>35</v>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
-        <v>82</v>
+      <c r="A20" s="18" t="s">
+        <v>83</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>35</v>
+      <c r="A21" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
-        <v>85</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add of argument range4boxplot in omic data importation plot functions
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\GitHub\DRomics\share\techdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182DE02C-4373-4B71-B07D-AD9A39A1FB4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0B67C6-D75C-4A72-8352-CBFE600AB279}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -247,9 +247,6 @@
     <t>28. Donner diverses options d’un plot de sensibilité par pathway (boxplot, autre stat résumées…) – fonction englobante sensitivityplot  avec plusieurs groupes (ex. article diuron) en résolvant le pb de l'ordre des items - FAIT EN PARTIE - A VALIDER PAR FLORIANE ET ELISE</t>
   </si>
   <si>
-    <t>33. Changer par défaut la représentation des boxplots des données pour qu’elle soit moins lourde (pour le moment géré juste avec range passé dans le … de la fonction plot</t>
-  </si>
-  <si>
     <t>37. Retravailler le modèle sigmoide, Lprobit et Gausprobit avec e = 0</t>
   </si>
   <si>
@@ -390,6 +387,12 @@
   </si>
   <si>
     <t>83. try to make the size scale of nb_of_items print only integer values in sensitivityplot and trendplot (cf. fig vignette 3.3) - pb ggplot</t>
+  </si>
+  <si>
+    <t>trop complexe</t>
+  </si>
+  <si>
+    <t>33. Changer par défaut la représentation des boxplots des données pour qu’elle soit moins lourde (pour le moment géré juste avec range passé dans le … de la fonction plot cf. point 61 fait</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -554,9 +557,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:B59"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1150,7 +1155,7 @@
     </row>
     <row r="44" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>35</v>
@@ -1158,7 +1163,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>51</v>
@@ -1166,7 +1171,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>35</v>
@@ -1174,7 +1179,7 @@
     </row>
     <row r="47" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -1182,7 +1187,7 @@
     </row>
     <row r="48" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>35</v>
@@ -1190,7 +1195,7 @@
     </row>
     <row r="49" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
         <v>35</v>
@@ -1198,7 +1203,7 @@
     </row>
     <row r="50" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>35</v>
@@ -1206,7 +1211,7 @@
     </row>
     <row r="51" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
         <v>35</v>
@@ -1214,7 +1219,7 @@
     </row>
     <row r="52" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>35</v>
@@ -1222,7 +1227,7 @@
     </row>
     <row r="53" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>35</v>
@@ -1230,7 +1235,7 @@
     </row>
     <row r="54" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>51</v>
@@ -1238,7 +1243,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>51</v>
@@ -1246,15 +1251,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>35</v>
@@ -1262,7 +1267,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>35</v>
@@ -1270,10 +1275,23 @@
     </row>
     <row r="59" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="17" t="s">
-        <v>97</v>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1284,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1324,6 +1342,9 @@
       <c r="B3" t="s">
         <v>35</v>
       </c>
+      <c r="D3" s="26" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
@@ -1349,7 +1370,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>53</v>
       </c>
@@ -1359,139 +1380,126 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>57</v>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>71</v>
+      <c r="A13" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
-        <v>89</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="21" t="s">
+        <v>94</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
-        <v>95</v>
+      <c r="A18" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>35</v>
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="21" t="s">
+      <c r="A20" s="21" t="s">
         <v>84</v>
       </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="21" t="s">
         <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1518,27 +1526,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1562,17 +1570,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of the TODO list and correcion of the defensive checks in bmdplotwithgradient (add of check on y0 and maxychange)
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\GitHub\DRomics\share\techdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0B67C6-D75C-4A72-8352-CBFE600AB279}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07155AFB-5866-4B6B-BBED-FBA1C8171FE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -356,18 +356,12 @@
     <t>84. ajouter dans le package une fonction de visualisation de l'ensemble des données en ACP pour voir la cohérence et détecter d'éventuels outliers</t>
   </si>
   <si>
-    <t>62. ajouter un test sur les outliers pour les cas excessifs cf. transcripto rainettes 2018 (implémenter sur chaque item, dès la vérification des données, sans prendre en compte la dose-réponse, une détection basée sur le Z-score modifié de Iglewicz, B., &amp; Hoaglin, D. C. (1993). How to detect and handle outliers (Vol. 16). Asq Press. (1115 citations google scholar)) - cf. point 84 lié</t>
-  </si>
-  <si>
     <t>70. look at the problem of format of the last page of the pdf file with the argument BMDoutput (cf. ex. transcripto 2018) - too complex !!!</t>
   </si>
   <si>
     <t>71. put an example to help the formating of data especially in a R object or write a function to do that from count matrix and dose</t>
   </si>
   <si>
-    <t>72. Transform sensitivityplot to return as an invisible object the numerical summaries and to do other plots (boxplots)</t>
-  </si>
-  <si>
     <t>ML puis A</t>
   </si>
   <si>
@@ -393,6 +387,15 @@
   </si>
   <si>
     <t>33. Changer par défaut la représentation des boxplots des données pour qu’elle soit moins lourde (pour le moment géré juste avec range passé dans le … de la fonction plot cf. point 61 fait</t>
+  </si>
+  <si>
+    <t>85. suivant</t>
+  </si>
+  <si>
+    <t>62. ajouter un test sur les outliers pour les cas excessifs cf. transcripto rainettes 2018 (implémenter sur chaque item, dès la vérification des données, sans prendre en compte la dose-réponse, une détection basée sur le Z-score modifié de Iglewicz, B., &amp; Hoaglin, D. C. (1993). How to detect and handle outliers (Vol. 16). Asq Press. (1115 citations google scholar)) - cf. point 84 lié et réglé en partie par choix de la méthode de transfo à vst si nb samples &gt; 30 (cf. Love)</t>
+  </si>
+  <si>
+    <t>72. Transform sensitivityplot to return as an invisible object the numerical summaries and to do other plots (boxplots) - impossible - write a function sensitivitycalc that will be called internally by sensitivityplot</t>
   </si>
 </sst>
 </file>
@@ -910,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1254,12 +1257,12 @@
         <v>79</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>35</v>
@@ -1267,7 +1270,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>35</v>
@@ -1275,10 +1278,10 @@
     </row>
     <row r="59" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1291,7 +1294,31 @@
     </row>
     <row r="61" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A63" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1302,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1343,7 +1370,7 @@
         <v>35</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1409,9 +1436,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>87</v>
+    <row r="13" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
@@ -1419,15 +1446,15 @@
     </row>
     <row r="14" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1435,66 +1462,47 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
-        <v>81</v>
+      <c r="A17" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>83</v>
+      <c r="A18" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" t="s">
-        <v>91</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the TODO list and add of a script to do the new figs for the updated cheat sheet
</commit_message>
<xml_diff>
--- a/share/techdoc/DRomicsTODOlist.xlsx
+++ b/share/techdoc/DRomicsTODOlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeligne\Documents\GitHub\DRomics\share\techdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07155AFB-5866-4B6B-BBED-FBA1C8171FE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24692D0A-84F9-480C-BDA2-BD6A22EE7626}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="105">
   <si>
     <t xml:space="preserve">task </t>
   </si>
@@ -389,13 +389,25 @@
     <t>33. Changer par défaut la représentation des boxplots des données pour qu’elle soit moins lourde (pour le moment géré juste avec range passé dans le … de la fonction plot cf. point 61 fait</t>
   </si>
   <si>
-    <t>85. suivant</t>
-  </si>
-  <si>
     <t>62. ajouter un test sur les outliers pour les cas excessifs cf. transcripto rainettes 2018 (implémenter sur chaque item, dès la vérification des données, sans prendre en compte la dose-réponse, une détection basée sur le Z-score modifié de Iglewicz, B., &amp; Hoaglin, D. C. (1993). How to detect and handle outliers (Vol. 16). Asq Press. (1115 citations google scholar)) - cf. point 84 lié et réglé en partie par choix de la méthode de transfo à vst si nb samples &gt; 30 (cf. Love)</t>
   </si>
   <si>
     <t>72. Transform sensitivityplot to return as an invisible object the numerical summaries and to do other plots (boxplots) - impossible - write a function sensitivitycalc that will be called internally by sensitivityplot</t>
+  </si>
+  <si>
+    <t>ML prototype in the share</t>
+  </si>
+  <si>
+    <t>85. add an example in the vignette where the need is obvious to work on log scale for bmdplot, sensitivity plot….</t>
+  </si>
+  <si>
+    <t>86. Add on the Dromics web page an introduction of the functions to help biological interpretation</t>
+  </si>
+  <si>
+    <t>87. change the figs in the cheat sheet using new options, new terminolgy in coherence to the one adopted in DRomicsIntepreter (biological group, experimental level) and add new functions</t>
+  </si>
+  <si>
+    <t>A et ML</t>
   </si>
 </sst>
 </file>
@@ -1329,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1438,7 +1450,7 @@
     </row>
     <row r="13" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
@@ -1454,7 +1466,7 @@
     </row>
     <row r="15" spans="1:4" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1465,7 +1477,7 @@
         <v>81</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1501,8 +1513,27 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
-        <v>98</v>
+      <c r="A21" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>